<commit_message>
01.11.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/October/All Details/28.10.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/October/All Details/28.10.2020/MC Bank Statement Sep-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Oct 2020" sheetId="7" r:id="rId1"/>
@@ -3113,6 +3113,15 @@
     <xf numFmtId="0" fontId="39" fillId="44" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="37" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3191,18 +3200,54 @@
     <xf numFmtId="2" fontId="39" fillId="35" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="39" fillId="35" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3214,51 +3259,6 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="11" fillId="43" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="35" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="39" fillId="35" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="39" fillId="37" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="55">
@@ -3351,7 +3351,7 @@
         <xdr:cNvPr id="1845" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47ED9286-E99E-4170-A6CD-A90D2E00B60F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3363,7 +3363,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3386,14 +3386,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3430,7 +3430,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3442,7 +3442,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3465,14 +3465,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -3849,21 +3849,21 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:8" ht="20.25">
-      <c r="B2" s="301" t="s">
+      <c r="B2" s="304" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="301"/>
-      <c r="D2" s="301"/>
-      <c r="E2" s="301"/>
+      <c r="C2" s="304"/>
+      <c r="D2" s="304"/>
+      <c r="E2" s="304"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1">
       <c r="A3" s="35"/>
-      <c r="B3" s="302" t="s">
+      <c r="B3" s="305" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
+      <c r="C3" s="305"/>
+      <c r="D3" s="305"/>
+      <c r="E3" s="305"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
       <c r="B4" s="36" t="s">
@@ -5021,7 +5021,7 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -5040,24 +5040,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="26.25">
-      <c r="A1" s="303" t="s">
+      <c r="A1" s="306" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="304"/>
-      <c r="C1" s="304"/>
-      <c r="D1" s="304"/>
-      <c r="E1" s="305"/>
+      <c r="B1" s="307"/>
+      <c r="C1" s="307"/>
+      <c r="D1" s="307"/>
+      <c r="E1" s="308"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:29" ht="23.25">
-      <c r="A2" s="306" t="s">
+      <c r="A2" s="309" t="s">
         <v>228</v>
       </c>
-      <c r="B2" s="307"/>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="308"/>
+      <c r="B2" s="310"/>
+      <c r="C2" s="310"/>
+      <c r="D2" s="310"/>
+      <c r="E2" s="311"/>
       <c r="F2" s="5"/>
       <c r="G2" s="11"/>
       <c r="H2" s="8"/>
@@ -5541,13 +5541,13 @@
       <c r="AC14" s="8"/>
     </row>
     <row r="15" spans="1:29" ht="22.5">
-      <c r="A15" s="309" t="s">
+      <c r="A15" s="312" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="310"/>
-      <c r="C15" s="310"/>
-      <c r="D15" s="310"/>
-      <c r="E15" s="311"/>
+      <c r="B15" s="313"/>
+      <c r="C15" s="313"/>
+      <c r="D15" s="313"/>
+      <c r="E15" s="314"/>
       <c r="F15" s="5"/>
       <c r="G15" s="9"/>
       <c r="H15" s="28"/>
@@ -10735,8 +10735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -10761,14 +10761,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:61" ht="19.5">
-      <c r="A1" s="318" t="s">
+      <c r="A1" s="321" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="318"/>
-      <c r="C1" s="318"/>
-      <c r="D1" s="318"/>
-      <c r="E1" s="318"/>
-      <c r="F1" s="318"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
       <c r="L1" s="104"/>
       <c r="M1" s="105"/>
       <c r="N1" s="105"/>
@@ -10821,14 +10821,14 @@
       <c r="BI1" s="105"/>
     </row>
     <row r="2" spans="1:61" ht="15">
-      <c r="A2" s="319" t="s">
+      <c r="A2" s="322" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="319"/>
-      <c r="C2" s="319"/>
-      <c r="D2" s="319"/>
-      <c r="E2" s="319"/>
-      <c r="F2" s="319"/>
+      <c r="B2" s="322"/>
+      <c r="C2" s="322"/>
+      <c r="D2" s="322"/>
+      <c r="E2" s="322"/>
+      <c r="F2" s="322"/>
       <c r="L2" s="104"/>
       <c r="M2" s="105"/>
       <c r="N2" s="105"/>
@@ -10881,14 +10881,14 @@
       <c r="BI2" s="105"/>
     </row>
     <row r="3" spans="1:61">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="323" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="320"/>
-      <c r="C3" s="320"/>
-      <c r="D3" s="320"/>
-      <c r="E3" s="320"/>
-      <c r="F3" s="320"/>
+      <c r="B3" s="323"/>
+      <c r="C3" s="323"/>
+      <c r="D3" s="323"/>
+      <c r="E3" s="323"/>
+      <c r="F3" s="323"/>
       <c r="K3" s="105"/>
       <c r="L3" s="104"/>
       <c r="M3" s="105"/>
@@ -13254,12 +13254,12 @@
       <c r="BI34" s="105"/>
     </row>
     <row r="35" spans="1:61" ht="12.6" customHeight="1" thickBot="1">
-      <c r="A35" s="321" t="s">
+      <c r="A35" s="324" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="322"/>
-      <c r="C35" s="322"/>
-      <c r="D35" s="323"/>
+      <c r="B35" s="325"/>
+      <c r="C35" s="325"/>
+      <c r="D35" s="326"/>
       <c r="E35" s="121"/>
       <c r="F35" s="123"/>
       <c r="G35" s="137"/>
@@ -13333,11 +13333,11 @@
       </c>
       <c r="E36" s="150">
         <f>F33-C113+K136</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="F36" s="151">
         <f>F33-C113-I43-I42+K136-C118</f>
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="G36" s="137"/>
       <c r="H36" s="145"/>
@@ -13403,7 +13403,7 @@
         <v>54</v>
       </c>
       <c r="C37" s="115">
-        <v>11720</v>
+        <v>11320</v>
       </c>
       <c r="D37" s="108" t="s">
         <v>227</v>
@@ -13834,13 +13834,13 @@
         <v>225</v>
       </c>
       <c r="E43" s="121"/>
-      <c r="F43" s="324" t="s">
+      <c r="F43" s="327" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="324"/>
-      <c r="H43" s="324"/>
-      <c r="I43" s="324"/>
-      <c r="J43" s="324"/>
+      <c r="G43" s="327"/>
+      <c r="H43" s="327"/>
+      <c r="I43" s="327"/>
+      <c r="J43" s="327"/>
       <c r="K43" s="168"/>
       <c r="L43" s="112"/>
       <c r="M43" s="105"/>
@@ -14904,10 +14904,10 @@
       <c r="BI58" s="105"/>
     </row>
     <row r="59" spans="1:61" ht="12" customHeight="1">
-      <c r="A59" s="325" t="s">
+      <c r="A59" s="328" t="s">
         <v>33</v>
       </c>
-      <c r="B59" s="326"/>
+      <c r="B59" s="329"/>
       <c r="C59" s="184"/>
       <c r="D59" s="188"/>
       <c r="E59" s="120"/>
@@ -15118,10 +15118,10 @@
         <v>164</v>
       </c>
       <c r="E62" s="129"/>
-      <c r="F62" s="312" t="s">
+      <c r="F62" s="315" t="s">
         <v>78</v>
       </c>
-      <c r="G62" s="312"/>
+      <c r="G62" s="315"/>
       <c r="H62" s="192"/>
       <c r="I62" s="192"/>
       <c r="J62" s="193" t="s">
@@ -17547,14 +17547,14 @@
       <c r="BI92" s="105"/>
     </row>
     <row r="93" spans="1:61" ht="14.25" customHeight="1">
-      <c r="A93" s="347" t="s">
+      <c r="A93" s="301" t="s">
         <v>229</v>
       </c>
-      <c r="B93" s="348"/>
-      <c r="C93" s="349">
+      <c r="B93" s="302"/>
+      <c r="C93" s="303">
         <v>820</v>
       </c>
-      <c r="D93" s="348" t="s">
+      <c r="D93" s="302" t="s">
         <v>227</v>
       </c>
       <c r="F93" s="203"/>
@@ -19050,13 +19050,13 @@
       <c r="BI112" s="105"/>
     </row>
     <row r="113" spans="1:61">
-      <c r="A113" s="313" t="s">
+      <c r="A113" s="316" t="s">
         <v>130</v>
       </c>
-      <c r="B113" s="314"/>
+      <c r="B113" s="317"/>
       <c r="C113" s="210">
         <f>SUM(C37:C112)</f>
-        <v>2366407</v>
+        <v>2366007</v>
       </c>
       <c r="D113" s="211"/>
       <c r="F113" s="203"/>
@@ -19195,13 +19195,13 @@
       <c r="BI114" s="105"/>
     </row>
     <row r="115" spans="1:61">
-      <c r="A115" s="315" t="s">
+      <c r="A115" s="318" t="s">
         <v>131</v>
       </c>
-      <c r="B115" s="316"/>
+      <c r="B115" s="319"/>
       <c r="C115" s="215">
         <f>C113+L136</f>
-        <v>2366407</v>
+        <v>2366007</v>
       </c>
       <c r="D115" s="216"/>
       <c r="F115" s="196"/>
@@ -21285,8 +21285,8 @@
       <c r="J169" s="104"/>
     </row>
     <row r="170" spans="5:13">
-      <c r="F170" s="317"/>
-      <c r="G170" s="317"/>
+      <c r="F170" s="320"/>
+      <c r="G170" s="320"/>
       <c r="H170" s="105"/>
       <c r="I170" s="127"/>
       <c r="J170" s="104"/>
@@ -21943,94 +21943,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="23.25">
-      <c r="A1" s="335" t="s">
+      <c r="A1" s="330" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="335"/>
-      <c r="C1" s="335"/>
-      <c r="D1" s="335"/>
-      <c r="E1" s="335"/>
-      <c r="F1" s="335"/>
-      <c r="G1" s="335"/>
-      <c r="H1" s="335"/>
-      <c r="I1" s="335"/>
-      <c r="J1" s="335"/>
-      <c r="K1" s="335"/>
-      <c r="L1" s="335"/>
-      <c r="M1" s="335"/>
-      <c r="N1" s="335"/>
-      <c r="O1" s="335"/>
-      <c r="P1" s="335"/>
-      <c r="Q1" s="335"/>
-      <c r="R1" s="335"/>
-      <c r="S1" s="335"/>
+      <c r="B1" s="330"/>
+      <c r="C1" s="330"/>
+      <c r="D1" s="330"/>
+      <c r="E1" s="330"/>
+      <c r="F1" s="330"/>
+      <c r="G1" s="330"/>
+      <c r="H1" s="330"/>
+      <c r="I1" s="330"/>
+      <c r="J1" s="330"/>
+      <c r="K1" s="330"/>
+      <c r="L1" s="330"/>
+      <c r="M1" s="330"/>
+      <c r="N1" s="330"/>
+      <c r="O1" s="330"/>
+      <c r="P1" s="330"/>
+      <c r="Q1" s="330"/>
+      <c r="R1" s="330"/>
+      <c r="S1" s="330"/>
     </row>
     <row r="2" spans="1:26" s="237" customFormat="1" ht="18">
-      <c r="A2" s="336" t="s">
+      <c r="A2" s="331" t="s">
         <v>132</v>
       </c>
-      <c r="B2" s="336"/>
-      <c r="C2" s="336"/>
-      <c r="D2" s="336"/>
-      <c r="E2" s="336"/>
-      <c r="F2" s="336"/>
-      <c r="G2" s="336"/>
-      <c r="H2" s="336"/>
-      <c r="I2" s="336"/>
-      <c r="J2" s="336"/>
-      <c r="K2" s="336"/>
-      <c r="L2" s="336"/>
-      <c r="M2" s="336"/>
-      <c r="N2" s="336"/>
-      <c r="O2" s="336"/>
-      <c r="P2" s="336"/>
-      <c r="Q2" s="336"/>
-      <c r="R2" s="336"/>
-      <c r="S2" s="336"/>
+      <c r="B2" s="331"/>
+      <c r="C2" s="331"/>
+      <c r="D2" s="331"/>
+      <c r="E2" s="331"/>
+      <c r="F2" s="331"/>
+      <c r="G2" s="331"/>
+      <c r="H2" s="331"/>
+      <c r="I2" s="331"/>
+      <c r="J2" s="331"/>
+      <c r="K2" s="331"/>
+      <c r="L2" s="331"/>
+      <c r="M2" s="331"/>
+      <c r="N2" s="331"/>
+      <c r="O2" s="331"/>
+      <c r="P2" s="331"/>
+      <c r="Q2" s="331"/>
+      <c r="R2" s="331"/>
+      <c r="S2" s="331"/>
     </row>
     <row r="3" spans="1:26" s="237" customFormat="1">
-      <c r="A3" s="337"/>
-      <c r="B3" s="337"/>
-      <c r="C3" s="337"/>
-      <c r="D3" s="337"/>
-      <c r="E3" s="337"/>
-      <c r="F3" s="337"/>
-      <c r="G3" s="337"/>
-      <c r="H3" s="337"/>
-      <c r="I3" s="337"/>
-      <c r="J3" s="337"/>
-      <c r="K3" s="337"/>
-      <c r="L3" s="337"/>
-      <c r="M3" s="337"/>
-      <c r="N3" s="337"/>
-      <c r="O3" s="337"/>
-      <c r="P3" s="337"/>
-      <c r="Q3" s="337"/>
-      <c r="R3" s="337"/>
-      <c r="S3" s="337"/>
+      <c r="A3" s="332"/>
+      <c r="B3" s="332"/>
+      <c r="C3" s="332"/>
+      <c r="D3" s="332"/>
+      <c r="E3" s="332"/>
+      <c r="F3" s="332"/>
+      <c r="G3" s="332"/>
+      <c r="H3" s="332"/>
+      <c r="I3" s="332"/>
+      <c r="J3" s="332"/>
+      <c r="K3" s="332"/>
+      <c r="L3" s="332"/>
+      <c r="M3" s="332"/>
+      <c r="N3" s="332"/>
+      <c r="O3" s="332"/>
+      <c r="P3" s="332"/>
+      <c r="Q3" s="332"/>
+      <c r="R3" s="332"/>
+      <c r="S3" s="332"/>
     </row>
     <row r="4" spans="1:26" s="238" customFormat="1" ht="16.5" thickBot="1">
-      <c r="A4" s="338" t="s">
+      <c r="A4" s="333" t="s">
         <v>189</v>
       </c>
-      <c r="B4" s="339"/>
-      <c r="C4" s="339"/>
-      <c r="D4" s="339"/>
-      <c r="E4" s="339"/>
-      <c r="F4" s="339"/>
-      <c r="G4" s="339"/>
-      <c r="H4" s="339"/>
-      <c r="I4" s="339"/>
-      <c r="J4" s="339"/>
-      <c r="K4" s="339"/>
-      <c r="L4" s="339"/>
-      <c r="M4" s="339"/>
-      <c r="N4" s="339"/>
-      <c r="O4" s="339"/>
-      <c r="P4" s="339"/>
-      <c r="Q4" s="339"/>
-      <c r="R4" s="339"/>
-      <c r="S4" s="340"/>
+      <c r="B4" s="334"/>
+      <c r="C4" s="334"/>
+      <c r="D4" s="334"/>
+      <c r="E4" s="334"/>
+      <c r="F4" s="334"/>
+      <c r="G4" s="334"/>
+      <c r="H4" s="334"/>
+      <c r="I4" s="334"/>
+      <c r="J4" s="334"/>
+      <c r="K4" s="334"/>
+      <c r="L4" s="334"/>
+      <c r="M4" s="334"/>
+      <c r="N4" s="334"/>
+      <c r="O4" s="334"/>
+      <c r="P4" s="334"/>
+      <c r="Q4" s="334"/>
+      <c r="R4" s="334"/>
+      <c r="S4" s="335"/>
       <c r="U4" s="121"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
@@ -22039,58 +22039,58 @@
       <c r="Z4" s="29"/>
     </row>
     <row r="5" spans="1:26" s="240" customFormat="1">
-      <c r="A5" s="341" t="s">
+      <c r="A5" s="336" t="s">
         <v>133</v>
       </c>
-      <c r="B5" s="343" t="s">
+      <c r="B5" s="338" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="329" t="s">
+      <c r="C5" s="340" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="329" t="s">
+      <c r="D5" s="340" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="329" t="s">
+      <c r="E5" s="340" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="329" t="s">
+      <c r="F5" s="340" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="329" t="s">
+      <c r="G5" s="340" t="s">
         <v>139</v>
       </c>
-      <c r="H5" s="329" t="s">
+      <c r="H5" s="340" t="s">
         <v>140</v>
       </c>
-      <c r="I5" s="329" t="s">
+      <c r="I5" s="340" t="s">
         <v>209</v>
       </c>
-      <c r="J5" s="329" t="s">
+      <c r="J5" s="340" t="s">
         <v>141</v>
       </c>
-      <c r="K5" s="329" t="s">
+      <c r="K5" s="340" t="s">
         <v>142</v>
       </c>
-      <c r="L5" s="329" t="s">
+      <c r="L5" s="340" t="s">
         <v>143</v>
       </c>
-      <c r="M5" s="329" t="s">
+      <c r="M5" s="340" t="s">
         <v>144</v>
       </c>
-      <c r="N5" s="329" t="s">
+      <c r="N5" s="340" t="s">
         <v>145</v>
       </c>
-      <c r="O5" s="331" t="s">
+      <c r="O5" s="346" t="s">
         <v>146</v>
       </c>
-      <c r="P5" s="333" t="s">
+      <c r="P5" s="348" t="s">
         <v>147</v>
       </c>
-      <c r="Q5" s="327" t="s">
+      <c r="Q5" s="344" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="345" t="s">
+      <c r="R5" s="342" t="s">
         <v>148</v>
       </c>
       <c r="S5" s="239" t="s">
@@ -22103,24 +22103,24 @@
       <c r="Y5" s="242"/>
     </row>
     <row r="6" spans="1:26" s="240" customFormat="1" ht="13.5" thickBot="1">
-      <c r="A6" s="342"/>
-      <c r="B6" s="344"/>
-      <c r="C6" s="330"/>
-      <c r="D6" s="330"/>
-      <c r="E6" s="330"/>
-      <c r="F6" s="330"/>
-      <c r="G6" s="330"/>
-      <c r="H6" s="330"/>
-      <c r="I6" s="330"/>
-      <c r="J6" s="330"/>
-      <c r="K6" s="330"/>
-      <c r="L6" s="330"/>
-      <c r="M6" s="330"/>
-      <c r="N6" s="330"/>
-      <c r="O6" s="332"/>
-      <c r="P6" s="334"/>
-      <c r="Q6" s="328"/>
-      <c r="R6" s="346"/>
+      <c r="A6" s="337"/>
+      <c r="B6" s="339"/>
+      <c r="C6" s="341"/>
+      <c r="D6" s="341"/>
+      <c r="E6" s="341"/>
+      <c r="F6" s="341"/>
+      <c r="G6" s="341"/>
+      <c r="H6" s="341"/>
+      <c r="I6" s="341"/>
+      <c r="J6" s="341"/>
+      <c r="K6" s="341"/>
+      <c r="L6" s="341"/>
+      <c r="M6" s="341"/>
+      <c r="N6" s="341"/>
+      <c r="O6" s="347"/>
+      <c r="P6" s="349"/>
+      <c r="Q6" s="345"/>
+      <c r="R6" s="343"/>
       <c r="S6" s="244" t="s">
         <v>149</v>
       </c>
@@ -25407,6 +25407,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="Q5:Q6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="O5:O6"/>
+    <mergeCell ref="P5:P6"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -25423,12 +25429,6 @@
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="Q5:Q6"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="P5:P6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>